<commit_message>
fix #72 sara re-check
</commit_message>
<xml_diff>
--- a/PLANNING/GANTT/GANTT.xlsx
+++ b/PLANNING/GANTT/GANTT.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="41">
   <si>
     <t>Mar
 </t>
@@ -23,29 +23,13 @@
     <t>May</t>
   </si>
   <si>
-    <t>Jun</t>
+    <t>June</t>
   </si>
   <si>
     <t>July</t>
   </si>
   <si>
-    <t>Aug</t>
-  </si>
-  <si>
     <t>Sept</t>
-  </si>
-  <si>
-    <t>Oct
-</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Dec</t>
-  </si>
-  <si>
-    <t>Jan</t>
   </si>
   <si>
     <t>Tasks</t>
@@ -107,7 +91,7 @@
     <t>Developing</t>
   </si>
   <si>
-    <t>10 Week</t>
+    <t>5 Week</t>
   </si>
   <si>
     <t>~40%</t>
@@ -116,7 +100,7 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>12 Week</t>
+    <t>6 Week</t>
   </si>
   <si>
     <t>~50%</t>
@@ -125,7 +109,7 @@
     <t>Operational</t>
   </si>
   <si>
-    <t>6 Week</t>
+    <t>3 Week</t>
   </si>
   <si>
     <t>~20%</t>
@@ -551,56 +535,46 @@
         <v>0</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F1" s="4"/>
       <c r="G1" s="3"/>
       <c r="H1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="J1" s="4"/>
       <c r="K1" s="3"/>
       <c r="L1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M1" s="3"/>
-      <c r="N1" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="N1" s="4"/>
       <c r="O1" s="3"/>
       <c r="P1" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q1" s="6"/>
-      <c r="R1" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="R1" s="4"/>
       <c r="S1" s="3"/>
       <c r="T1" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="U1" s="6"/>
-      <c r="V1" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="V1" s="4"/>
       <c r="W1" s="3"/>
       <c r="X1" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y1" s="6"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D2" s="10">
         <v>15.0</v>
@@ -671,37 +645,37 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" s="14">
         <v>42793.0</v>
       </c>
       <c r="C3" s="15">
-        <v>42915.0</v>
+        <v>42853.0</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -720,28 +694,28 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" s="14">
         <v>42793.0</v>
       </c>
       <c r="C4" s="15">
-        <v>42853.0</v>
+        <v>42832.0</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -763,22 +737,22 @@
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="14">
         <v>42793.0</v>
       </c>
       <c r="C5" s="15">
-        <v>42839.0</v>
+        <v>42818.0</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -802,19 +776,19 @@
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" s="14">
-        <v>42842.0</v>
+        <v>42821.0</v>
       </c>
       <c r="C6" s="15">
-        <v>42846.0</v>
+        <v>42825.0</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="21"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -837,20 +811,20 @@
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="14">
-        <v>42849.0</v>
+        <v>42828.0</v>
       </c>
       <c r="C7" s="15">
-        <v>42853.0</v>
+        <v>42832.0</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -872,33 +846,33 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="14">
-        <v>42828.0</v>
+        <v>42814.0</v>
       </c>
       <c r="C8" s="15">
-        <v>42915.0</v>
+        <v>42853.0</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
@@ -917,33 +891,33 @@
     </row>
     <row r="9">
       <c r="A9" s="20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="14">
-        <v>42828.0</v>
+        <v>42814.0</v>
       </c>
       <c r="C9" s="15">
-        <v>42916.0</v>
+        <v>42853.0</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
@@ -962,37 +936,37 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="14">
         <v>42793.0</v>
       </c>
       <c r="C10" s="15">
-        <v>42915.0</v>
+        <v>42853.0</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
@@ -1011,37 +985,37 @@
     </row>
     <row r="11">
       <c r="A11" s="20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="14">
-        <v>42798.0</v>
+        <v>42793.0</v>
       </c>
       <c r="C11" s="15">
-        <v>42920.0</v>
+        <v>42853.0</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
@@ -1060,13 +1034,13 @@
     </row>
     <row r="12">
       <c r="A12" s="20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" s="14">
-        <v>42799.0</v>
+        <v>42835.0</v>
       </c>
       <c r="C12" s="15">
-        <v>42921.0</v>
+        <v>42853.0</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -1074,13 +1048,13 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
@@ -1126,13 +1100,13 @@
     </row>
     <row r="14">
       <c r="A14" s="22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="14">
-        <v>42919.0</v>
+        <v>42856.0</v>
       </c>
       <c r="C14" s="15">
-        <v>43133.0</v>
+        <v>42986.0</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -1143,57 +1117,57 @@
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
       <c r="L14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="O14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="R14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="S14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="V14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="W14" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="X14" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Y14" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -1204,19 +1178,19 @@
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
       <c r="L15" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="O15" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="P15" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Q15" s="21"/>
       <c r="R15" s="21"/>
@@ -1229,13 +1203,13 @@
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -1251,22 +1225,22 @@
       <c r="O16" s="21"/>
       <c r="P16" s="21"/>
       <c r="Q16" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="R16" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="S16" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="T16" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="U16" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="V16" s="20" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
@@ -1274,13 +1248,13 @@
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -1301,22 +1275,22 @@
       <c r="T17" s="21"/>
       <c r="U17" s="21"/>
       <c r="W17" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="X17" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="Y17" s="18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="28">
-        <v>42993.0</v>
+        <v>42895.0</v>
       </c>
       <c r="D18" s="29"/>
       <c r="E18" s="19"/>
@@ -1331,7 +1305,7 @@
       <c r="N18" s="19"/>
       <c r="O18" s="19"/>
       <c r="P18" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="18"/>
@@ -1345,11 +1319,11 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B19" s="31"/>
       <c r="C19" s="28">
-        <v>43406.0</v>
+        <v>43280.0</v>
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="19"/>
@@ -1367,7 +1341,7 @@
       <c r="Q19" s="19"/>
       <c r="R19" s="19"/>
       <c r="S19" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
@@ -1378,11 +1352,11 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="28">
-        <v>43434.0</v>
+        <v>43308.0</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="19"/>
@@ -1403,7 +1377,7 @@
       <c r="T20" s="19"/>
       <c r="U20" s="19"/>
       <c r="V20" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="W20" s="19"/>
       <c r="X20" s="19"/>
@@ -1411,7 +1385,7 @@
     </row>
     <row r="21">
       <c r="A21" s="20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="32"/>
@@ -1440,7 +1414,7 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="28">
@@ -1468,7 +1442,7 @@
       <c r="W22" s="19"/>
       <c r="X22" s="19"/>
       <c r="Y22" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -1525,13 +1499,13 @@
     </row>
     <row r="25">
       <c r="B25" s="34" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
@@ -1557,13 +1531,13 @@
     </row>
     <row r="26">
       <c r="B26" s="34" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
@@ -1589,13 +1563,13 @@
     </row>
     <row r="27">
       <c r="B27" s="34" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>

</xml_diff>